<commit_message>
Change tables to reflect updated spec
</commit_message>
<xml_diff>
--- a/docs/spec/tables/keywords.xlsx
+++ b/docs/spec/tables/keywords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goats\Documents\dsl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goats\Documents\repos\cs3423-project\docs\spec\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93CD9516-D13B-4245-97FC-5CD84E44FCC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538ECDD8-2782-4E2B-9295-7BB165708891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{80D8C4F5-3D34-44DF-B7D6-9FF257957546}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>AND</t>
   </si>
@@ -53,9 +53,6 @@
     <t>IF</t>
   </si>
   <si>
-    <t>PI</t>
-  </si>
-  <si>
     <t>INT</t>
   </si>
   <si>
@@ -77,18 +74,12 @@
     <t>PROD</t>
   </si>
   <si>
-    <t>IMPORT</t>
-  </si>
-  <si>
     <t>DOUBLE</t>
   </si>
   <si>
     <t>BREAK</t>
   </si>
   <si>
-    <t>NROWS</t>
-  </si>
-  <si>
     <t>WHILE</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>CONTINUE</t>
   </si>
   <si>
-    <t>NCOLS</t>
-  </si>
-  <si>
     <t>FUN</t>
   </si>
   <si>
@@ -119,9 +107,6 @@
     <t>MAIN</t>
   </si>
   <si>
-    <t>NCELLS</t>
-  </si>
-  <si>
     <t>VOID</t>
   </si>
   <si>
@@ -129,6 +114,24 @@
   </si>
   <si>
     <t>FORMULA</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>POW</t>
+  </si>
+  <si>
+    <t>FLOOR</t>
+  </si>
+  <si>
+    <t>CEIL</t>
   </si>
 </sst>
 </file>
@@ -536,12 +539,13 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="12.6328125" style="1"/>
+    <col min="1" max="6" width="15.6328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="12.6328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -549,105 +553,105 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>29</v>
@@ -655,7 +659,9 @@
       <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update specification tables and examples
</commit_message>
<xml_diff>
--- a/docs/spec/tables/keywords.xlsx
+++ b/docs/spec/tables/keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goats\Documents\repos\cs3423-project\docs\spec\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46956F5C-42D7-4A21-A31B-5605D5038D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19AFA08-384F-499D-AEEC-BE94A8AF04BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{80D8C4F5-3D34-44DF-B7D6-9FF257957546}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>AND</t>
   </si>
@@ -56,9 +56,6 @@
     <t>INT</t>
   </si>
   <si>
-    <t>RETURNS</t>
-  </si>
-  <si>
     <t>SUM</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>TABLE</t>
   </si>
   <si>
-    <t>INF</t>
-  </si>
-  <si>
     <t>PROD</t>
   </si>
   <si>
@@ -110,9 +104,6 @@
     <t>VOID</t>
   </si>
   <si>
-    <t>GET</t>
-  </si>
-  <si>
     <t>FORMULA</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
   </si>
   <si>
     <t>FLOOR</t>
-  </si>
-  <si>
-    <t>CEIL</t>
   </si>
   <si>
     <t>BAND</t>
@@ -553,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAA00F9-1958-4299-BCCE-66D9004F88FB}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -570,7 +558,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
@@ -579,128 +567,112 @@
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update specification and examples
</commit_message>
<xml_diff>
--- a/docs/spec/tables/keywords.xlsx
+++ b/docs/spec/tables/keywords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goats\Documents\repos\cs3423-project\docs\spec\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goats\Documents\excel_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19AFA08-384F-499D-AEEC-BE94A8AF04BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6544F8D-843F-4492-B4D2-7465B76C4C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{80D8C4F5-3D34-44DF-B7D6-9FF257957546}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>VOID</t>
   </si>
   <si>
-    <t>FORMULA</t>
-  </si>
-  <si>
     <t>MUL</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>BLS</t>
+  </si>
+  <si>
+    <t>MODULUS</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -558,7 +558,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -588,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
@@ -611,7 +611,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -631,7 +631,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -651,27 +651,27 @@
         <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>